<commit_message>
Added first experiments to the paper.
</commit_message>
<xml_diff>
--- a/doc/Manuscript/data/precision.xlsx
+++ b/doc/Manuscript/data/precision.xlsx
@@ -103,6 +103,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,6 +136,1154 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'precision.csv'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'precision.csv'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Bubblesort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FloatMM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>IntMM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Oscar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RealMM</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Towers</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Treesort</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'precision.csv'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>30.232558</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.054054</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.158416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89.61039</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>66.666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.983607</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.516129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.571429</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.833333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>595.251583</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'precision.csv'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'precision.csv'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Bubblesort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FloatMM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>IntMM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Oscar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RealMM</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Towers</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Treesort</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'precision.csv'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.380952</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.639344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.020296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'precision.csv'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n*n</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'precision.csv'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Bubblesort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FloatMM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>IntMM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Oscar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RealMM</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Towers</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Treesort</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'precision.csv'!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>27.906977</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.980198</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.229508</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.333333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>89.450016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'precision.csv'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>imprecise</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'precision.csv'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Bubblesort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FloatMM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>IntMM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Oscar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RealMM</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Towers</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Treesort</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'precision.csv'!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>41.860465</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45.945946</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.861386</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.38961</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.952381</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31.147541</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.483871</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>71.42857100000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.833333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>411.278104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="455666296"/>
+        <c:axId val="451476312"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="455666296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="451476312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="451476312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="455666296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'precision.csv'!$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'precision.csv'!$A$16:$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Bubblesort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FloatMM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>IntMM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Oscar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RealMM</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Towers</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Treesort</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'precision.csv'!$B$16:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>16.27907</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.054054</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.50495</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.833333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.012987</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71.42857100000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.065574</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.516129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.714286</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.833333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>571.867287</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'precision.csv'!$C$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'precision.csv'!$A$16:$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Bubblesort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FloatMM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>IntMM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Oscar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RealMM</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Towers</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Treesort</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'precision.csv'!$C$16:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.910891</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.557377</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.468268</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'precision.csv'!$D$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n*n</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'precision.csv'!$A$16:$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Bubblesort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FloatMM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>IntMM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Oscar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RealMM</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Towers</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Treesort</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'precision.csv'!$D$16:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>20.930233</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.918919</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.920792</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.393443</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.580645</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.583333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>123.202365</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'precision.csv'!$E$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>imprecise</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'precision.csv'!$A$16:$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Bubblesort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FloatMM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>IntMM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Oscar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RealMM</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Towers</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Treesort</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'precision.csv'!$E$16:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>62.790698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.027027</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.663366</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.166667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.987013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.571429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.983607</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.903226</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64.285714</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64.583333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>389.46208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="460019112"/>
+        <c:axId val="533066360"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="460019112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533066360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="533066360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="460019112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1077,7 +2226,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Polished the paper a little bit.
</commit_message>
<xml_diff>
--- a/doc/Manuscript/data/precision.xlsx
+++ b/doc/Manuscript/data/precision.xlsx
@@ -85,12 +85,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -615,11 +609,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="455666296"/>
-        <c:axId val="451476312"/>
+        <c:axId val="483197608"/>
+        <c:axId val="483193208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455666296"/>
+        <c:axId val="483197608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,19 +624,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1000"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451476312"/>
+        <c:crossAx val="483193208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="451476312"/>
+        <c:axId val="483193208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,7 +644,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="455666296"/>
+        <c:crossAx val="483197608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1157,11 +1151,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="460019112"/>
-        <c:axId val="533066360"/>
+        <c:axId val="521196744"/>
+        <c:axId val="483369800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="460019112"/>
+        <c:axId val="521196744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1172,19 +1166,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1000"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533066360"/>
+        <c:crossAx val="483369800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533066360"/>
+        <c:axId val="483369800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1192,7 +1186,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="460019112"/>
+        <c:crossAx val="521196744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1227,8 +1221,8 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
@@ -1257,8 +1251,8 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
@@ -1609,7 +1603,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E27"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2224,6 +2218,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>